<commit_message>
bring latest template and SHS changes
</commit_message>
<xml_diff>
--- a/output/SharedHealthSummary/composition-shs-1.xlsx
+++ b/output/SharedHealthSummary/composition-shs-1.xlsx
@@ -1414,7 +1414,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-cmp-1:A section must at least one of text, entries, or sub-sections {text.exists() or entry.exists() or section.exists()}cmp-2:A section can only have an emptyReason if it is empty {emptyReason.empty() or entry.empty()}inv-dh-cmp-05:This section shall not contain both summary statements of medical history entries (condition or procedure) and assertions of no relevant finding entries {Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').exists() implies ((Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').entry.resolve().where($this is Condition).exists() or Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').entry.resolve().where($this is Procedure).exists()) xor Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').entry.resolve().where($this is Observation).exists())}inv-dh-cmp-06:This section shall contain at most one assertion of no relevant finding entry and it shall assert no relevant medical history {Composition.section.where($this.code.coding.system = 'https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').entry.resolve().where($this is Observation).exists() implies (Composition.section.where($this.code.coding.system = 'https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').entry.resolve().where($this is Observation).count()&lt;2 and Composition.section.where($this.code.coding.system = 'https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').entry.resolve().where($this is value and value.coding.code = '1224831000168103').exists())}</t>
+cmp-1:A section must at least one of text, entries, or sub-sections {text.exists() or entry.exists() or section.exists()}cmp-2:A section can only have an emptyReason if it is empty {emptyReason.empty() or entry.empty()}inv-dh-cmp-05:This section shall not contain both summary statement of medical history entries (condition or procedure) and assertion of no relevant finding entries {Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').exists() implies ((Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').entry.resolve().where($this is Condition).exists() or Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').entry.resolve().where($this is Procedure).exists()) xor Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').entry.resolve().where($this is Observation).exists())}inv-dh-cmp-06:This section shall contain at most one assertion of no relevant finding entry and it shall assert no relevant medical history {Composition.section.where($this.code.coding.system = 'https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').entry.resolve().where($this is Observation).exists() implies (Composition.section.where($this.code.coding.system = 'https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').entry.resolve().where($this is Observation).count()&lt;2 and Composition.section.where($this.code.coding.system = 'https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.16117').entry.resolve().where($this is value and value.coding.code = '1224831000168103').exists())}</t>
   </si>
   <si>
     <t>&lt;valueString xmlns="http://hl7.org/fhir" value="Medical History"/&gt;</t>
@@ -1445,7 +1445,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-cmp-1:A section must at least one of text, entries, or sub-sections {text.exists() or entry.exists() or section.exists()}cmp-2:A section can only have an emptyReason if it is empty {emptyReason.empty() or entry.empty()}inv-dh-cmp-07:This section shall not contain both summary statements of administered vaccine entries and assertions of no relevant finding entries {Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').exists() implies (Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is Immunization).exists() xor Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is Observation ).exists())}inv-dh-cmp-08:This section shall contain at most one assertion of no relevant finding entry and it shall assert no previous immunisations {Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is Observation).exists() implies (Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is Observation).count()&lt;2 and Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is value and value.coding.code = '401179006').exists())}</t>
+cmp-1:A section must at least one of text, entries, or sub-sections {text.exists() or entry.exists() or section.exists()}cmp-2:A section can only have an emptyReason if it is empty {emptyReason.empty() or entry.empty()}inv-dh-cmp-07:This section shall not contain both summary statement of administered vaccine entries and assertion of no relevant finding entries {Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').exists() implies (Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is Immunization).exists() xor Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is Observation ).exists())}inv-dh-cmp-08:This section shall contain at most one assertion of no relevant finding entry and it shall assert no previous immunisations {Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is Observation).exists() implies (Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is Observation).count()&lt;2 and Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is value and value.coding.code = '1234401000168109').exists())}</t>
   </si>
   <si>
     <t>&lt;valueString xmlns="http://hl7.org/fhir" value="Immunisations"/&gt;</t>

</xml_diff>

<commit_message>
updated SHS mappinsgs, and other minor changes
</commit_message>
<xml_diff>
--- a/output/SharedHealthSummary/composition-shs-1.xlsx
+++ b/output/SharedHealthSummary/composition-shs-1.xlsx
@@ -306,7 +306,7 @@
     <t>Profiles this resource claims to conform to</t>
   </si>
   <si>
-    <t>A list of profiles (references to [StructureDefinition](structuredefinition.html#) resources) that this resource claims to conform to. The URL is a reference to [StructureDefinition.url]().</t>
+    <t>A list of profiles (references to [StructureDefinition](https://build.fhir.org/ig/hl7au/au-fhir-base/structuredefinition.html#) resources) that this resource claims to conform to. The URL is a reference to [StructureDefinition.url](https://build.fhir.org/ig/hl7au/au-fhir-base/).</t>
   </si>
   <si>
     <t>It is up to the server and/or other infrastructure of policy to determine whether/how these claims are verified and/or updated over time.  The list of profile URLs is a set.</t>
@@ -1383,7 +1383,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-cmp-1:A section must at least one of text, entries, or sub-sections {text.exists() or entry.exists() or section.exists()}cmp-2:A section can only have an emptyReason if it is empty {emptyReason.empty() or entry.empty()}inv-dh-cmp-03:This section shall not contain both summary statement of known medication entries and assertion of no relevant finding entries {Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.32009').exists() implies (Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.32009').entry.resolve().where($this is MedicationStatement).exists() xor Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.32009').entry.resolve().where($this is Observation ).exists())}inv-dh-cmp-04:This section shall contain at most one assertion of no relevant finding entry and it shall assert no current medications {Composition.section.where($this.code.coding.system = 'https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.32009').entry.resolve().where($this is Observation).exists() implies (Composition.section.where($this.code.coding.system = 'https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.32009').entry.resolve().where($this is Observation).count()&lt;2 and Composition.section.where($this.code.coding.system = 'https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.32009').entry.resolve().where($this is value and value.coding.code = '1200661000168107').exists())}</t>
+cmp-1:A section must at least one of text, entries, or sub-sections {text.exists() or entry.exists() or section.exists()}cmp-2:A section can only have an emptyReason if it is empty {emptyReason.empty() or entry.empty()}inv-dh-cmp-03:This section shall not contain both summary statement of known medication entries and assertion of no relevant finding entries {Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.32009').exists() implies (Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.32009').entry.resolve().where($this is MedicationStatement).exists() xor Composition.section.where($this.code.coding.system='https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.32009').entry.resolve().where($this is Observation ).exists())}inv-dh-cmp-04:This section shall contain at most one assertion of no relevant finding entry and it shall assert no known current medications {Composition.section.where($this.code.coding.system = 'https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.32009').entry.resolve().where($this is Observation).exists() implies (Composition.section.where($this.code.coding.system = 'https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.32009').entry.resolve().where($this is Observation).count()&lt;2 and Composition.section.where($this.code.coding.system = 'https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1' and $this.code.coding.code = '101.32009').entry.resolve().where($this is value and value.coding.code = '1200661000168107').exists())}</t>
   </si>
   <si>
     <t>&lt;valueString xmlns="http://hl7.org/fhir" value="Current Medications"/&gt;</t>
@@ -1445,7 +1445,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-cmp-1:A section must at least one of text, entries, or sub-sections {text.exists() or entry.exists() or section.exists()}cmp-2:A section can only have an emptyReason if it is empty {emptyReason.empty() or entry.empty()}inv-dh-cmp-07:This section shall not contain both summary statement of administered vaccine entries and assertion of no relevant finding entries {Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').exists() implies (Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is Immunization).exists() xor Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is Observation ).exists())}inv-dh-cmp-08:This section shall contain at most one assertion of no relevant finding entry and it shall assert no previous immunisations {Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is Observation).exists() implies (Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is Observation).count()&lt;2 and Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is value and value.coding.code = '1234401000168109').exists())}</t>
+cmp-1:A section must at least one of text, entries, or sub-sections {text.exists() or entry.exists() or section.exists()}cmp-2:A section can only have an emptyReason if it is empty {emptyReason.empty() or entry.empty()}inv-dh-cmp-07:This section shall not contain both summary statement of administered vaccine entries and assertion of no relevant finding entries {Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').exists() implies (Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is Immunization).exists() xor Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is Observation ).exists())}inv-dh-cmp-08:This section shall contain at most one assertion of no relevant finding entry and it shall assert no history of vaccination {Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is Observation).exists() implies (Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is Observation).count()&lt;2 and Composition.section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '11369-6').entry.resolve().where($this is value and value.coding.code = '1234401000168109').exists())}</t>
   </si>
   <si>
     <t>&lt;valueString xmlns="http://hl7.org/fhir" value="Immunisations"/&gt;</t>

</xml_diff>